<commit_message>
Extent report support added
</commit_message>
<xml_diff>
--- a/SeleniumTestNGFramework/src/config/testdata.xlsx
+++ b/SeleniumTestNGFramework/src/config/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\SeleniumTestNGFramework\src\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sures\git\SELENIUM_JAVA_TESTNG\SeleniumTestNGFramework\src\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DCE5C5-500C-46C6-8E30-8A77484947AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384FB789-74FB-4DAB-A957-7547698382FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A69F248D-EA57-451B-BCB3-24FF285435D4}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>ESS</t>
   </si>
   <si>
-    <t>John Smith</t>
-  </si>
-  <si>
     <t>Enabled</t>
   </si>
   <si>
@@ -57,20 +54,29 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
-    <t>Test003Qa</t>
+    <t>Abc15033</t>
+  </si>
+  <si>
+    <t>Steven Edwards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF5D5D5D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,12 +419,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -439,30 +446,31 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>